<commit_message>
xlsx update on 8-15
</commit_message>
<xml_diff>
--- a/调用资料/pystudy2.xlsx
+++ b/调用资料/pystudy2.xlsx
@@ -1,37 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\pyNote\调用资料\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PythonStudy_Git\调用资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E0DACA-3926-4E1B-B7EB-CD4128CDA987}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE83671-6E61-4E2C-9970-D1A4BE0FDE97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="690" windowWidth="19365" windowHeight="14910" xr2:uid="{AC7E9008-9A35-4319-AC7A-327ED70E26E9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{AC7E9008-9A35-4319-AC7A-327ED70E26E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="38">
   <si>
     <t>内容</t>
   </si>
@@ -137,6 +132,18 @@
   </si>
   <si>
     <t>内容分类</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>材料</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>柚子酱</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -521,7 +528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9C719AA-DEDF-42F0-BCE9-216999A7899C}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -953,4 +960,37 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C38867A-2DA5-4DCD-B6A0-71AA7D512C0E}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>